<commit_message>
included functions for generating zip file
</commit_message>
<xml_diff>
--- a/backend/api/Book.xlsx
+++ b/backend/api/Book.xlsx
@@ -20,33 +20,21 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="9">
-  <si>
-    <t xml:space="preserve">UserId</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Username</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DId</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DName</t>
-  </si>
-  <si>
-    <t xml:space="preserve">vyshnav</t>
-  </si>
-  <si>
-    <t xml:space="preserve">adasd</t>
-  </si>
-  <si>
-    <t xml:space="preserve">asdasd</t>
-  </si>
-  <si>
-    <t xml:space="preserve">zameel</t>
-  </si>
-  <si>
-    <t xml:space="preserve">asdasdasd</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+  <si>
+    <t xml:space="preserve">GSTIN</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NAME</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Vyshnav Raj</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Zameel</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Name3</t>
   </si>
 </sst>
 </file>
@@ -122,8 +110,12 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -152,10 +144,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D5" activeCellId="0" sqref="D5"/>
+      <selection pane="topLeft" activeCell="E11" activeCellId="0" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -170,59 +162,38 @@
       <c r="B1" s="0" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="0" t="s">
+    </row>
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="1" t="n">
+        <v>123456789</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="0" t="s">
+      <c r="C2" s="2"/>
+      <c r="D2" s="2"/>
+    </row>
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="n">
+        <v>237411212</v>
+      </c>
+      <c r="B3" s="0" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="B2" s="0" t="s">
+      <c r="C3" s="3"/>
+      <c r="D3" s="3"/>
+    </row>
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="n">
+        <v>29487023894</v>
+      </c>
+      <c r="B4" s="0" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C3" s="2" t="n">
-        <v>2</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C4" s="2" t="n">
-        <v>3</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="n">
-        <v>2</v>
-      </c>
-      <c r="B5" s="0" t="s">
-        <v>7</v>
-      </c>
-      <c r="D5" s="0" t="s">
-        <v>8</v>
-      </c>
+      <c r="C4" s="3"/>
+      <c r="D4" s="3"/>
     </row>
   </sheetData>
-  <mergeCells count="2">
-    <mergeCell ref="A2:A4"/>
-    <mergeCell ref="B2:B4"/>
-  </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
   <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>

</xml_diff>